<commit_message>
Testing implementation of "Single Author Customized query"
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\DBLPTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\publication-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A680D5-D620-4577-A987-102DAC7D4101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A87B8B2-4BE9-4DC1-AD6F-DC0057C5B448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{731FB0E4-0319-429C-B671-FE074528AF85}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{731FB0E4-0319-429C-B671-FE074528AF85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Emna Rbii</t>
+  </si>
+  <si>
+    <t>Robert Schifreen</t>
   </si>
 </sst>
 </file>
@@ -418,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF172AAA-820B-4879-8790-0659C49DE76D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,6 +497,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>